<commit_message>
adding 2 modified files
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Assignment for submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CCS_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9391DED2-1D91-47A8-9EB4-7D2101174082}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD5FF9F-99DD-4182-8E1B-DD671B3051DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="63">
   <si>
     <t>Task</t>
   </si>
@@ -213,13 +213,19 @@
   </si>
   <si>
     <t>- 6-Sep</t>
+  </si>
+  <si>
+    <t>two week</t>
+  </si>
+  <si>
+    <t>Testing Environment Training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +237,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -269,7 +282,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="7" tint="0.59996337778862885"/>
       </patternFill>
     </fill>
@@ -446,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -547,24 +560,31 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -651,6 +671,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
@@ -685,6 +712,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="9" tint="-0.24994659260841701"/>
@@ -702,6 +739,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
@@ -714,6 +758,33 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
@@ -994,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,8 +1240,8 @@
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
@@ -1252,7 +1323,7 @@
         <v>43644</v>
       </c>
       <c r="F8" s="3" t="str">
-        <f t="shared" ref="F8:Q40" si="2">IF(AND(F$4&gt;=$D8,F$4&lt;=$E8),"X","")</f>
+        <f t="shared" ref="F8:Q41" si="2">IF(AND(F$4&gt;=$D8,F$4&lt;=$E8),"X","")</f>
         <v>X</v>
       </c>
       <c r="G8" s="3" t="str">
@@ -2440,7 +2511,7 @@
         <v/>
       </c>
       <c r="O26" s="3" t="str">
-        <f t="shared" ref="G26:Q40" si="9">IF(AND(O$4&gt;=$D26,O$4&lt;=$E26),"X","")</f>
+        <f t="shared" ref="G26:Q41" si="9">IF(AND(O$4&gt;=$D26,O$4&lt;=$E26),"X","")</f>
         <v/>
       </c>
       <c r="P26" s="48" t="str">
@@ -2837,329 +2908,329 @@
       </c>
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="41">
+      <c r="A33" s="42"/>
+      <c r="B33" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="56">
+        <f>D32</f>
+        <v>43675</v>
+      </c>
+      <c r="E33" s="57">
+        <f>E32+11</f>
+        <v>43690</v>
+      </c>
+      <c r="F33" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>X</v>
+      </c>
+      <c r="M33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>X</v>
+      </c>
+      <c r="N33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v>X</v>
+      </c>
+      <c r="O33" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P33" s="46" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q33" s="46" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="41">
         <v>6</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B34" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="K33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="L33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="N33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="O33" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="P33" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Q33" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
-      <c r="B34" s="35" t="s">
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O34" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P34" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q34" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="42"/>
+      <c r="B35" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C35" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="37">
-        <f>E32+3</f>
-        <v>43682</v>
-      </c>
-      <c r="E34" s="37">
-        <f>D34+4</f>
-        <v>43686</v>
-      </c>
-      <c r="F34" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="K34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="L34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M34" s="3" t="str">
+      <c r="D35" s="37">
+        <f>E33+3</f>
+        <v>43693</v>
+      </c>
+      <c r="E35" s="37">
+        <f>D35+4</f>
+        <v>43697</v>
+      </c>
+      <c r="F35" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N35" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O35" s="3" t="str">
         <f t="shared" si="9"/>
         <v>X</v>
       </c>
-      <c r="N34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="O34" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="P34" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Q34" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="41">
+      <c r="P35" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q35" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="41">
         <v>7</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B36" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="K35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="L35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="N35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="O35" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="P35" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Q35" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="35" t="s">
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="27" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O36" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P36" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q36" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="42"/>
+      <c r="B37" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C37" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D36" s="37">
-        <f>E34+3</f>
-        <v>43689</v>
-      </c>
-      <c r="E36" s="37">
-        <f>D36+4</f>
-        <v>43693</v>
-      </c>
-      <c r="F36" s="3" t="str">
-        <f>IF(AND(F$4&gt;=$D36,F$4&lt;=$E36),"X","")</f>
-        <v/>
-      </c>
-      <c r="G36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="K36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="L36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="N36" s="3" t="str">
+      <c r="D37" s="37">
+        <f>E35+3</f>
+        <v>43700</v>
+      </c>
+      <c r="E37" s="37">
+        <f>D37+4</f>
+        <v>43704</v>
+      </c>
+      <c r="F37" s="3" t="str">
+        <f>IF(AND(F$4&gt;=$D37,F$4&lt;=$E37),"X","")</f>
+        <v/>
+      </c>
+      <c r="G37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O37" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P37" s="48" t="str">
         <f t="shared" si="9"/>
         <v>X</v>
       </c>
-      <c r="O36" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="P36" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Q36" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="41">
+      <c r="Q37" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="41">
         <v>8</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B38" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="K37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="L37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="N37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="O37" s="3" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="P37" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Q37" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="5">
-        <f>E36+3</f>
-        <v>43696</v>
-      </c>
-      <c r="E38" s="5">
-        <f>D38+4</f>
-        <v>43700</v>
-      </c>
-      <c r="F38" s="3" t="str">
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="27" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
@@ -3197,7 +3268,7 @@
       </c>
       <c r="O38" s="3" t="str">
         <f t="shared" si="9"/>
-        <v>X</v>
+        <v/>
       </c>
       <c r="P38" s="48" t="str">
         <f t="shared" si="9"/>
@@ -3210,19 +3281,19 @@
     </row>
     <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="42"/>
-      <c r="B39" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="3">
-        <f>D38</f>
-        <v>43696</v>
+      <c r="D39" s="5">
+        <f>E37+3</f>
+        <v>43707</v>
       </c>
       <c r="E39" s="5">
         <f>D39+4</f>
-        <v>43700</v>
+        <v>43711</v>
       </c>
       <c r="F39" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3262,116 +3333,198 @@
       </c>
       <c r="O39" s="3" t="str">
         <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P39" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q39" s="48" t="str">
+        <f t="shared" si="9"/>
         <v>X</v>
       </c>
-      <c r="P39" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="Q39" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
     </row>
     <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
-      <c r="B40" s="46" t="s">
+      <c r="A40" s="42"/>
+      <c r="B40" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D40" s="3">
+        <f>D39</f>
+        <v>43707</v>
+      </c>
+      <c r="E40" s="5">
+        <f>D40+4</f>
+        <v>43711</v>
+      </c>
+      <c r="F40" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O40" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P40" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="Q40" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v>X</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="50"/>
+      <c r="B41" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C40" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="48">
-        <f>E39+3</f>
+      <c r="C41" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="48">
         <v>43703</v>
       </c>
-      <c r="E40" s="49">
-        <f>D40+11</f>
+      <c r="E41" s="53">
+        <f>D41+11</f>
         <v>43714</v>
       </c>
-      <c r="F40" s="48" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="G40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="H40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="I40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="J40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="K40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="L40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="N40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="O40" s="48" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="P40" s="50" t="str">
-        <f t="shared" si="9"/>
-        <v>X</v>
-      </c>
-      <c r="Q40" s="50" t="str">
-        <f t="shared" si="9"/>
-        <v>X</v>
-      </c>
+      <c r="F41" s="48" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="H41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="J41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="K41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="L41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="M41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="N41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="O41" s="48" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="P41" s="49"/>
+      <c r="Q41" s="49"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F6:O39">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+  <conditionalFormatting sqref="F6:O32 F34:O40">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="18" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F40:O40">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+  <conditionalFormatting sqref="F41:O41">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="16" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P6:P39">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+  <conditionalFormatting sqref="P6:P32 P34:P40">
+    <cfRule type="cellIs" dxfId="19" priority="13" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="14" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P40">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+  <conditionalFormatting sqref="P41">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"X"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q6:Q39">
+  <conditionalFormatting sqref="Q6:Q32 Q34:Q40">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q41">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F33:O33">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P33">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"X"</formula>
     </cfRule>
@@ -3379,7 +3532,7 @@
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q40">
+  <conditionalFormatting sqref="Q33">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"X"</formula>
     </cfRule>

</xml_diff>